<commit_message>
création sommaire de l'interface XML chooseTrainingActivity
</commit_message>
<xml_diff>
--- a/Programme.xlsx
+++ b/Programme.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72ab51e9346d1936/Documents/INSA/Projet/Appli fracationnée/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programme_secondaire\CODE\Fractionne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{686E4101-6754-4D4B-B523-78DBD8B11205}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{DF3E9FAC-712F-47EE-8E22-D6DE38F91D9B}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{8DC4F982-F149-4638-9C25-F71187E5D791}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -101,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -284,7 +283,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -305,50 +308,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -664,354 +663,359 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9D5E5C-3984-40F6-960E-D8AC7BF97AD6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65:D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.1328125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="33.4" x14ac:dyDescent="0.45">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-    </row>
-    <row r="2" spans="2:16" ht="33.4" x14ac:dyDescent="0.45">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+    </row>
+    <row r="2" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="2:16" ht="33.4" x14ac:dyDescent="0.45">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="2:16" ht="33.4" x14ac:dyDescent="0.45">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="F5" s="11" t="s">
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="K5" s="13" t="s">
+      <c r="G5" s="14"/>
+      <c r="K5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="K7" s="13"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="K8" s="13"/>
-    </row>
-    <row r="10" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="1">
-      <c r="B10" s="14" t="s">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="10" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B15" s="4" t="s">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="21"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="21"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="21"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B17" s="4" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B19" s="4" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B21" s="4" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B23" s="4" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B25" s="4" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B30" s="23" t="s">
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B33" s="4" t="s">
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B35" s="4" t="s">
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B37" s="4" t="s">
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B41" s="18" t="s">
+      <c r="C37" s="7"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="11"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B46" s="18" t="s">
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B52" s="18" t="s">
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="F52" s="10"/>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B56" s="18" t="s">
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B60" s="18" t="s">
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B1:D4"/>
+    <mergeCell ref="H1:J4"/>
+    <mergeCell ref="N1:P4"/>
+    <mergeCell ref="B10:D14"/>
+    <mergeCell ref="B15:D16"/>
     <mergeCell ref="B52:D54"/>
     <mergeCell ref="B56:D58"/>
     <mergeCell ref="B60:D62"/>
@@ -1028,11 +1032,6 @@
     <mergeCell ref="B23:D24"/>
     <mergeCell ref="B41:D43"/>
     <mergeCell ref="B30:D32"/>
-    <mergeCell ref="B1:D4"/>
-    <mergeCell ref="H1:J4"/>
-    <mergeCell ref="N1:P4"/>
-    <mergeCell ref="B10:D14"/>
-    <mergeCell ref="B15:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Création de l'activity : create fractionne
</commit_message>
<xml_diff>
--- a/Programme.xlsx
+++ b/Programme.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -284,28 +284,55 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -322,33 +349,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65:D67"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20:P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,362 +676,362 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
     </row>
     <row r="4" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="K5" s="5" t="s">
+      <c r="G5" s="23"/>
+      <c r="K5" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="K6" s="5"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="K7" s="5"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="K8" s="5"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="22"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="21"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="22"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="21"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="22"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
+      <c r="N14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="15"/>
+      <c r="P14" s="16"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="19"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+      <c r="N16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+      <c r="O16" s="15"/>
+      <c r="P16" s="16"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N17" s="17"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="19"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+      <c r="O18" s="15"/>
+      <c r="P18" s="16"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N19" s="17"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="19"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N20" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="O20" s="15"/>
+      <c r="P20" s="16"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N21" s="17"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="19"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H23" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+      <c r="I23" s="15"/>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H24" s="17"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="19"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H25" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="15" t="s">
+      <c r="I25" s="15"/>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H26" s="17"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="11"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="19"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="16"/>
     </row>
     <row r="36" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="19"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="16"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="11"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="19"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
       <c r="F52" s="3"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B1:D4"/>
-    <mergeCell ref="H1:J4"/>
-    <mergeCell ref="N1:P4"/>
-    <mergeCell ref="B10:D14"/>
-    <mergeCell ref="B15:D16"/>
     <mergeCell ref="B52:D54"/>
     <mergeCell ref="B56:D58"/>
     <mergeCell ref="B60:D62"/>
     <mergeCell ref="K5:K8"/>
-    <mergeCell ref="B25:D26"/>
+    <mergeCell ref="H25:J26"/>
     <mergeCell ref="B33:D34"/>
     <mergeCell ref="B35:D36"/>
     <mergeCell ref="B37:D38"/>
     <mergeCell ref="B46:D49"/>
     <mergeCell ref="F5:G8"/>
-    <mergeCell ref="B17:D18"/>
-    <mergeCell ref="B19:D20"/>
-    <mergeCell ref="B21:D22"/>
-    <mergeCell ref="B23:D24"/>
+    <mergeCell ref="N16:P17"/>
+    <mergeCell ref="N18:P19"/>
+    <mergeCell ref="N20:P21"/>
+    <mergeCell ref="H23:J24"/>
     <mergeCell ref="B41:D43"/>
     <mergeCell ref="B30:D32"/>
+    <mergeCell ref="B1:D4"/>
+    <mergeCell ref="H1:J4"/>
+    <mergeCell ref="N1:P4"/>
+    <mergeCell ref="H9:J13"/>
+    <mergeCell ref="N14:P15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Excel : Creation activité XML done
</commit_message>
<xml_diff>
--- a/Programme.xlsx
+++ b/Programme.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>A faire</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Seance in progress</t>
+  </si>
+  <si>
+    <t>Creation activité test</t>
   </si>
 </sst>
 </file>
@@ -277,41 +280,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -330,9 +309,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -348,6 +324,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -664,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P62"/>
+  <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20:P21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,362 +697,375 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
     </row>
     <row r="2" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
     </row>
     <row r="3" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
     </row>
     <row r="4" spans="2:16" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="K5" s="20" t="s">
+      <c r="G5" s="14"/>
+      <c r="K5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="K6" s="20"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="K7" s="20"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="K8" s="20"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H9" s="5" t="s">
+      <c r="N9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="20"/>
     </row>
     <row r="10" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
       <c r="M10" s="1"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="22"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="22"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="22"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="13"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="25"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N14" s="14" t="s">
+      <c r="N14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="O14" s="15"/>
-      <c r="P14" s="16"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N15" s="17"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="19"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="11"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N16" s="14" t="s">
+      <c r="N16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="O16" s="15"/>
-      <c r="P16" s="16"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N17" s="17"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="19"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N18" s="14" t="s">
+      <c r="O16" s="7"/>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N17" s="9"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="11"/>
+    </row>
+    <row r="18" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O18" s="15"/>
-      <c r="P18" s="16"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N19" s="17"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="19"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="14" t="s">
+      <c r="O18" s="7"/>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N19" s="9"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="11"/>
+    </row>
+    <row r="20" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="O20" s="15"/>
-      <c r="P20" s="16"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="N21" s="17"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="19"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H23" s="14" t="s">
+      <c r="O20" s="7"/>
+      <c r="P20" s="8"/>
+    </row>
+    <row r="21" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N21" s="9"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="11"/>
+    </row>
+    <row r="22" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="15"/>
-      <c r="J23" s="16"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H24" s="17"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="19"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H25" s="14" t="s">
+      <c r="O22" s="7"/>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N23" s="9"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="11"/>
+    </row>
+    <row r="24" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N24" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="16"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H26" s="17"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="19"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="24" t="s">
+      <c r="O24" s="7"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="N25" s="9"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="11"/>
+    </row>
+    <row r="29" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H29" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+    </row>
+    <row r="31" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+    </row>
+    <row r="32" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H32" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="26"/>
+      <c r="J32" s="29"/>
+    </row>
+    <row r="33" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="30"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="31"/>
+    </row>
+    <row r="34" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="16"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="17"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="19"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
+      <c r="I34" s="7"/>
+      <c r="J34" s="8"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H35" s="9"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="11"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H36" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="16"/>
-    </row>
-    <row r="36" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="19"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
+      <c r="I36" s="7"/>
+      <c r="J36" s="8"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H37" s="9"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="16"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="19"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="9" t="s">
+      <c r="I38" s="7"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H39" s="9"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="11"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="9" t="s">
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="9" t="s">
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B52:D54"/>
-    <mergeCell ref="B56:D58"/>
-    <mergeCell ref="B60:D62"/>
-    <mergeCell ref="K5:K8"/>
-    <mergeCell ref="H25:J26"/>
-    <mergeCell ref="B33:D34"/>
-    <mergeCell ref="B35:D36"/>
-    <mergeCell ref="B37:D38"/>
-    <mergeCell ref="B46:D49"/>
-    <mergeCell ref="F5:G8"/>
+  <mergeCells count="22">
+    <mergeCell ref="B1:D4"/>
+    <mergeCell ref="H1:J4"/>
+    <mergeCell ref="N1:P4"/>
+    <mergeCell ref="N9:P13"/>
+    <mergeCell ref="N14:P15"/>
     <mergeCell ref="N16:P17"/>
     <mergeCell ref="N18:P19"/>
     <mergeCell ref="N20:P21"/>
-    <mergeCell ref="H23:J24"/>
-    <mergeCell ref="B41:D43"/>
-    <mergeCell ref="B30:D32"/>
-    <mergeCell ref="B1:D4"/>
-    <mergeCell ref="H1:J4"/>
-    <mergeCell ref="N1:P4"/>
-    <mergeCell ref="H9:J13"/>
-    <mergeCell ref="N14:P15"/>
+    <mergeCell ref="N22:P23"/>
+    <mergeCell ref="B43:D45"/>
+    <mergeCell ref="H29:J31"/>
+    <mergeCell ref="H32:J33"/>
+    <mergeCell ref="B54:D56"/>
+    <mergeCell ref="B58:D60"/>
+    <mergeCell ref="B62:D64"/>
+    <mergeCell ref="K5:K8"/>
+    <mergeCell ref="N24:P25"/>
+    <mergeCell ref="H34:J35"/>
+    <mergeCell ref="H36:J37"/>
+    <mergeCell ref="H38:J39"/>
+    <mergeCell ref="B48:D51"/>
+    <mergeCell ref="F5:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>